<commit_message>
Atualiza modelo e reformula código para checar a existência dos arquivos necessários
</commit_message>
<xml_diff>
--- a/modelo_calendario.xlsx
+++ b/modelo_calendario.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\CSV to Google Calendar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\csv_to_google_calendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CC091C-8EDC-479D-9131-FD3D9BE8282F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A6F494-DCB2-40DB-BD0D-EA66B21C444B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>Subject</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Private</t>
   </si>
   <si>
-    <t>Reunião Teste</t>
-  </si>
-  <si>
     <t>04/13/2022</t>
   </si>
   <si>
@@ -65,13 +62,22 @@
   </si>
   <si>
     <t>TRUE</t>
+  </si>
+  <si>
+    <t>Reunião Teste 1</t>
+  </si>
+  <si>
+    <t>Reunião Teste 2</t>
+  </si>
+  <si>
+    <t>Reunião Teste 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +208,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -548,9 +562,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -906,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,80 +970,84 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
       </c>
       <c r="C2" s="1">
         <v>0.63194444444444442</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1">
         <v>0.66666666666666663</v>
       </c>
       <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
       </c>
       <c r="C3" s="1">
         <v>0.67361111111111116</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1">
         <v>0.70833333333333337</v>
       </c>
       <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
-      </c>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>